<commit_message>
added 4 more data points
</commit_message>
<xml_diff>
--- a/experiment/data.xlsx
+++ b/experiment/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uchicagoedu-my.sharepoint.com/personal/wtchen_uchicago_edu/Documents/uchicago-fourthyear/HCI/project1/hci-project1/experiment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="8_{C47ECC5B-F132-6644-BEBC-EC0B35DF3B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF8908A6-A2CF-AB40-B0C0-96ABE274EFF1}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="8_{C47ECC5B-F132-6644-BEBC-EC0B35DF3B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1F760FA-5FDA-49E6-84A8-A2F59114BB02}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17120" xr2:uid="{021E2D31-30A6-8444-98B7-74580109CCA6}"/>
+    <workbookView xWindow="29580" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{021E2D31-30A6-8444-98B7-74580109CCA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -62,10 +60,25 @@
     <t>Additional notes</t>
   </si>
   <si>
-    <t>James</t>
-  </si>
-  <si>
     <t>Understood how to perform the gestures intuitively after the experiment finished.</t>
+  </si>
+  <si>
+    <t>James Kenniff</t>
+  </si>
+  <si>
+    <t>Kiki Apple</t>
+  </si>
+  <si>
+    <t>Max Gallo</t>
+  </si>
+  <si>
+    <t>Used the hard punch to clear his picture without instruction</t>
+  </si>
+  <si>
+    <t>Andy Yang</t>
+  </si>
+  <si>
+    <t>Andy Liu</t>
   </si>
 </sst>
 </file>
@@ -127,10 +140,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -430,24 +439,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0D3074D-7E25-EB4C-AB39-D1484D7770F0}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="39" customWidth="1"/>
-    <col min="3" max="3" width="43.1640625" customWidth="1"/>
-    <col min="4" max="4" width="36.6640625" customWidth="1"/>
-    <col min="5" max="5" width="51.83203125" customWidth="1"/>
-    <col min="6" max="6" width="28.1640625" customWidth="1"/>
+    <col min="3" max="3" width="43.125" customWidth="1"/>
+    <col min="4" max="4" width="36.625" customWidth="1"/>
+    <col min="5" max="5" width="51.875" customWidth="1"/>
+    <col min="6" max="6" width="28.125" customWidth="1"/>
     <col min="7" max="7" width="25.5" customWidth="1"/>
-    <col min="8" max="8" width="54.83203125" customWidth="1"/>
+    <col min="8" max="8" width="54.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -473,9 +483,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>7</v>
@@ -496,7 +506,102 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
         <v>9</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>